<commit_message>
improved test with parallel run
</commit_message>
<xml_diff>
--- a/RestaurantApp/src/test/resources/datacontroller/RestaurantAppController.xlsx
+++ b/RestaurantApp/src/test/resources/datacontroller/RestaurantAppController.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14670" windowHeight="6075" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14670" windowHeight="6075"/>
   </bookViews>
   <sheets>
     <sheet name="headless" sheetId="3" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="UserInput" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I18"/>
+  <oleSize ref="A1:H18"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -118,13 +118,13 @@
     <t>Serial</t>
   </si>
   <si>
+    <t>sushi</t>
+  </si>
+  <si>
+    <t>vincent</t>
+  </si>
+  <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>sushi</t>
-  </si>
-  <si>
-    <t>vincent</t>
   </si>
 </sst>
 </file>
@@ -504,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,7 +528,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,7 +668,7 @@
         <v>8888</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
@@ -679,7 +679,7 @@
         <v>8888</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>